<commit_message>
Adding more sample datasets
</commit_message>
<xml_diff>
--- a/sample-data/iris-data.xlsx
+++ b/sample-data/iris-data.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/sarahkaiser_microsoft_com/Documents/Desktop/snakes-in-a-grid/sample-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{42DE7B46-E250-49F9-BBE3-A6F25EE2287E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B93F949-FDAC-4A63-9916-702FBE7C47F4}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{42DE7B46-E250-49F9-BBE3-A6F25EE2287E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31BD3CAC-8940-4874-89E1-1AE14045A485}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="997" yWindow="1920" windowWidth="21600" windowHeight="11333" activeTab="1" xr2:uid="{FE88425F-BCD3-41E7-A99D-D84B8BED82F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{FE88425F-BCD3-41E7-A99D-D84B8BED82F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Iris" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,18 +50,11 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="2">
+  <futureMetadata name="XLRICHVALUE" count="1">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="3"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="4"/>
         </ext>
       </extLst>
     </bk>
@@ -73,12 +64,9 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="2">
+  <valueMetadata count="1">
     <bk>
       <rc t="2" v="0"/>
-    </bk>
-    <bk>
-      <rc t="2" v="1"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -109,11 +97,6 @@
 categories = sample_df["species"].unique()  # Get unique categories
 colors = {category: i for i, category in enumerate(categories)}
 scatter_matrix(sample_df, c=sample_df["species"].apply(lambda x: colors[x]), figsize=(6, 6), alpha=0.8)</code>
-    </pythonScript>
-    <pythonScript>
-      <code xml:space="preserve">import faker
-faker.help
-</code>
     </pythonScript>
   </pythonScripts>
 </python>
@@ -326,8 +309,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6257925" y="2895600"/>
-          <a:ext cx="5214937" cy="2055812"/>
+          <a:off x="6138333" y="2947654"/>
+          <a:ext cx="5116160" cy="2091600"/>
           <a:chOff x="6257925" y="2895600"/>
           <a:chExt cx="5214937" cy="2055812"/>
         </a:xfrm>
@@ -600,7 +583,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
   <rv s="0">
     <v>0</v>
     <v>9</v>
@@ -617,22 +600,15 @@
   <rv s="3">
     <v>&lt;class 'PIL.PngImagePlugin.PngImageFile'&gt;</v>
     <v>PngImageFile</v>
-    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=521x529 at 0x7F4731CEF650&gt;</v>
+    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=521x529 at 0x7FEBF67C8560&gt;</v>
     <v>2</v>
-    <v>1</v>
-  </rv>
-  <rv s="4">
-    <v>5dcd32950dc046bcb44f75b17f86bc2e</v>
-    <v>module 'faker' has no attribute 'help'</v>
-    <v>AttributeError</v>
-    <v>18</v>
     <v>1</v>
   </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
   <s t="_localImage">
     <k n="_rvRel:LocalImageIdentifier" t="i"/>
     <k n="CalcOrigin" t="i"/>
@@ -652,13 +628,6 @@
     <k n="Python_str" t="s"/>
     <k n="preview" t="r"/>
     <k n="_Provider" t="spb"/>
-  </s>
-  <s t="_error">
-    <k n="correlationId" t="s"/>
-    <k n="errorMessage" t="s"/>
-    <k n="errorName" t="s"/>
-    <k n="errorType" t="i"/>
-    <k n="subType" t="i"/>
   </s>
 </rvStructures>
 </file>
@@ -1074,22 +1043,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8714A0-714B-49DD-96CA-E07F9F991C76}">
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="11" width="14.59765625" customWidth="1"/>
+    <col min="1" max="11" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1110,7 +1079,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5.0999999999999996</v>
       </c>
@@ -1131,7 +1100,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4.9000000000000004</v>
       </c>
@@ -1148,7 +1117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4.7</v>
       </c>
@@ -1166,7 +1135,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4.5999999999999996</v>
       </c>
@@ -1183,7 +1152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1200,7 +1169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5.4</v>
       </c>
@@ -1217,7 +1186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4.5999999999999996</v>
       </c>
@@ -1234,7 +1203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1251,7 +1220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4.4000000000000004</v>
       </c>
@@ -1268,7 +1237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>4.9000000000000004</v>
       </c>
@@ -1285,7 +1254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5.4</v>
       </c>
@@ -1302,7 +1271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>4.8</v>
       </c>
@@ -1319,7 +1288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>4.8</v>
       </c>
@@ -1336,7 +1305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>4.3</v>
       </c>
@@ -1353,7 +1322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5.8</v>
       </c>
@@ -1370,7 +1339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5.7</v>
       </c>
@@ -1387,7 +1356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>5.4</v>
       </c>
@@ -1404,7 +1373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>5.0999999999999996</v>
       </c>
@@ -1421,7 +1390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>5.7</v>
       </c>
@@ -1438,7 +1407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>5.0999999999999996</v>
       </c>
@@ -1455,7 +1424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>5.4</v>
       </c>
@@ -1472,7 +1441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>5.0999999999999996</v>
       </c>
@@ -1489,7 +1458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>4.5999999999999996</v>
       </c>
@@ -1506,7 +1475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>5.0999999999999996</v>
       </c>
@@ -1523,7 +1492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>4.8</v>
       </c>
@@ -1540,7 +1509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>5</v>
       </c>
@@ -1557,7 +1526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1574,7 +1543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>5.2</v>
       </c>
@@ -1591,7 +1560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>5.2</v>
       </c>
@@ -1608,7 +1577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>4.7</v>
       </c>
@@ -1625,7 +1594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>4.8</v>
       </c>
@@ -1642,7 +1611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>5.4</v>
       </c>
@@ -1659,7 +1628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>5.2</v>
       </c>
@@ -1676,7 +1645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>5.5</v>
       </c>
@@ -1693,7 +1662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4.9000000000000004</v>
       </c>
@@ -1710,7 +1679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
@@ -1727,7 +1696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5.5</v>
       </c>
@@ -1744,7 +1713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>4.9000000000000004</v>
       </c>
@@ -1761,7 +1730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>4.4000000000000004</v>
       </c>
@@ -1778,7 +1747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>5.0999999999999996</v>
       </c>
@@ -1795,7 +1764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>5</v>
       </c>
@@ -1812,7 +1781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>4.5</v>
       </c>
@@ -1829,7 +1798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>4.4000000000000004</v>
       </c>
@@ -1846,7 +1815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>5</v>
       </c>
@@ -1863,7 +1832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>5.0999999999999996</v>
       </c>
@@ -1880,7 +1849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>4.8</v>
       </c>
@@ -1897,7 +1866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>5.0999999999999996</v>
       </c>
@@ -1914,7 +1883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>4.5999999999999996</v>
       </c>
@@ -1931,7 +1900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>5.3</v>
       </c>
@@ -1948,7 +1917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>5</v>
       </c>
@@ -1965,7 +1934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>7</v>
       </c>
@@ -1982,7 +1951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>6.4</v>
       </c>
@@ -1999,7 +1968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>6.9</v>
       </c>
@@ -2016,7 +1985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>5.5</v>
       </c>
@@ -2033,7 +2002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>6.5</v>
       </c>
@@ -2050,7 +2019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>5.7</v>
       </c>
@@ -2067,7 +2036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>6.3</v>
       </c>
@@ -2084,7 +2053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>4.9000000000000004</v>
       </c>
@@ -2101,7 +2070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>6.6</v>
       </c>
@@ -2118,7 +2087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>5.2</v>
       </c>
@@ -2135,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>5</v>
       </c>
@@ -2152,7 +2121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>5.9</v>
       </c>
@@ -2169,7 +2138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>6</v>
       </c>
@@ -2186,7 +2155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>6.1</v>
       </c>
@@ -2203,7 +2172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>5.6</v>
       </c>
@@ -2220,7 +2189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>6.7</v>
       </c>
@@ -2237,7 +2206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>5.6</v>
       </c>
@@ -2254,7 +2223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>5.8</v>
       </c>
@@ -2271,7 +2240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>6.2</v>
       </c>
@@ -2288,7 +2257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>5.6</v>
       </c>
@@ -2305,7 +2274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>5.9</v>
       </c>
@@ -2322,7 +2291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>6.1</v>
       </c>
@@ -2339,7 +2308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>6.3</v>
       </c>
@@ -2356,7 +2325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>6.1</v>
       </c>
@@ -2373,7 +2342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>6.4</v>
       </c>
@@ -2390,7 +2359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>6.6</v>
       </c>
@@ -2407,7 +2376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>6.8</v>
       </c>
@@ -2424,7 +2393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>6.7</v>
       </c>
@@ -2441,7 +2410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>6</v>
       </c>
@@ -2458,7 +2427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>5.7</v>
       </c>
@@ -2475,7 +2444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>5.5</v>
       </c>
@@ -2492,7 +2461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>5.5</v>
       </c>
@@ -2509,7 +2478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>5.8</v>
       </c>
@@ -2526,7 +2495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>6</v>
       </c>
@@ -2543,7 +2512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>5.4</v>
       </c>
@@ -2560,7 +2529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>6</v>
       </c>
@@ -2577,7 +2546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>6.7</v>
       </c>
@@ -2594,7 +2563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>6.3</v>
       </c>
@@ -2611,7 +2580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>5.6</v>
       </c>
@@ -2628,7 +2597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>5.5</v>
       </c>
@@ -2645,7 +2614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>5.5</v>
       </c>
@@ -2662,7 +2631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>6.1</v>
       </c>
@@ -2679,7 +2648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>5.8</v>
       </c>
@@ -2696,7 +2665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>5</v>
       </c>
@@ -2713,7 +2682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>5.6</v>
       </c>
@@ -2730,7 +2699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>5.7</v>
       </c>
@@ -2747,7 +2716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>5.7</v>
       </c>
@@ -2764,7 +2733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>6.2</v>
       </c>
@@ -2781,7 +2750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>5.0999999999999996</v>
       </c>
@@ -2798,7 +2767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>5.7</v>
       </c>
@@ -2815,7 +2784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>6.3</v>
       </c>
@@ -2832,7 +2801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>5.8</v>
       </c>
@@ -2849,7 +2818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>7.1</v>
       </c>
@@ -2866,7 +2835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>6.3</v>
       </c>
@@ -2883,7 +2852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>6.5</v>
       </c>
@@ -2900,7 +2869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>7.6</v>
       </c>
@@ -2917,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>4.9000000000000004</v>
       </c>
@@ -2934,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>7.3</v>
       </c>
@@ -2951,7 +2920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>6.7</v>
       </c>
@@ -2968,7 +2937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>7.2</v>
       </c>
@@ -2985,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>6.5</v>
       </c>
@@ -3002,7 +2971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>6.4</v>
       </c>
@@ -3019,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>6.8</v>
       </c>
@@ -3036,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>5.7</v>
       </c>
@@ -3053,7 +3022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>5.8</v>
       </c>
@@ -3070,7 +3039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>6.4</v>
       </c>
@@ -3087,7 +3056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>6.5</v>
       </c>
@@ -3104,7 +3073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>7.7</v>
       </c>
@@ -3121,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>7.7</v>
       </c>
@@ -3138,7 +3107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>6</v>
       </c>
@@ -3155,7 +3124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>6.9</v>
       </c>
@@ -3172,7 +3141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>5.6</v>
       </c>
@@ -3189,7 +3158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>7.7</v>
       </c>
@@ -3206,7 +3175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>6.3</v>
       </c>
@@ -3223,7 +3192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>6.7</v>
       </c>
@@ -3240,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>7.2</v>
       </c>
@@ -3257,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>6.2</v>
       </c>
@@ -3274,7 +3243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>6.1</v>
       </c>
@@ -3291,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>6.4</v>
       </c>
@@ -3308,7 +3277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>7.2</v>
       </c>
@@ -3325,7 +3294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>7.4</v>
       </c>
@@ -3342,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>7.9</v>
       </c>
@@ -3359,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>6.4</v>
       </c>
@@ -3376,7 +3345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>6.3</v>
       </c>
@@ -3393,7 +3362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>6.1</v>
       </c>
@@ -3410,7 +3379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>7.7</v>
       </c>
@@ -3427,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>6.3</v>
       </c>
@@ -3444,7 +3413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>6.4</v>
       </c>
@@ -3461,7 +3430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>6</v>
       </c>
@@ -3478,7 +3447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>6.9</v>
       </c>
@@ -3495,7 +3464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>6.7</v>
       </c>
@@ -3512,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>6.9</v>
       </c>
@@ -3529,7 +3498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>5.8</v>
       </c>
@@ -3546,7 +3515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>6.8</v>
       </c>
@@ -3563,7 +3532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>6.7</v>
       </c>
@@ -3580,7 +3549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>6.7</v>
       </c>
@@ -3597,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>6.3</v>
       </c>
@@ -3614,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>6.5</v>
       </c>
@@ -3631,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>6.2</v>
       </c>
@@ -3648,7 +3617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>5.9</v>
       </c>
@@ -3665,7 +3634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>0</v>
       </c>
@@ -3679,25 +3648,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DBEC57-6D71-49C5-95E0-2E3F959F8558}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" t="e" cm="1" vm="2">
-        <f t="array" ref="A1">_xlfn._xlws.PY(1,1)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>